<commit_message>
add material manage function
</commit_message>
<xml_diff>
--- a/doc/MenuFormat.xlsx
+++ b/doc/MenuFormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="10755" windowHeight="6930" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="10755" windowHeight="6930" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Category1" sheetId="1" r:id="rId1"/>
@@ -17,20 +17,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="48">
   <si>
     <t>ID</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Chinese_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>English_Name</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sequence</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -204,6 +196,17 @@
   </si>
   <si>
     <t>5. Dish里面的hotLevel, 取值范围0-3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstLanguage_Name</t>
+  </si>
+  <si>
+    <t>SecondLanguage_Name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FirstLanguage_Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -551,13 +554,13 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="17.875" customWidth="1"/>
-    <col min="3" max="3" width="16.25" customWidth="1"/>
+    <col min="2" max="2" width="20.125" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
     <col min="4" max="4" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -566,13 +569,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>47</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -580,10 +583,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -594,10 +597,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -614,13 +617,13 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="16.75" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="3" max="3" width="21" customWidth="1"/>
     <col min="4" max="4" width="13.125" customWidth="1"/>
     <col min="5" max="5" width="15.625" customWidth="1"/>
   </cols>
@@ -630,16 +633,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -647,10 +650,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -664,10 +667,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -681,10 +684,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -698,10 +701,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -720,14 +723,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="2" max="2" width="16.875" customWidth="1"/>
-    <col min="3" max="3" width="17.375" customWidth="1"/>
+    <col min="2" max="2" width="21.75" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
     <col min="4" max="4" width="13.875" customWidth="1"/>
     <col min="5" max="5" width="14.625" customWidth="1"/>
   </cols>
@@ -737,28 +740,28 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -766,10 +769,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" t="s">
         <v>32</v>
-      </c>
-      <c r="C2" t="s">
-        <v>34</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -795,10 +798,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
         <v>33</v>
-      </c>
-      <c r="C3" t="s">
-        <v>35</v>
       </c>
       <c r="D3">
         <v>2</v>
@@ -824,10 +827,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D4">
         <v>1</v>
@@ -853,10 +856,10 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>2</v>
@@ -882,10 +885,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6">
         <v>1</v>
@@ -911,10 +914,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -940,10 +943,10 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D8">
         <v>1</v>
@@ -969,10 +972,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D9">
         <v>2</v>
@@ -998,10 +1001,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D10">
         <v>3</v>
@@ -1027,10 +1030,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D11">
         <v>3</v>
@@ -1061,7 +1064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
@@ -1072,27 +1075,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>